<commit_message>
pipenv changed excel updated
</commit_message>
<xml_diff>
--- a/Selenium_Training/Excel/moneydata.xlsx
+++ b/Selenium_Training/Excel/moneydata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,10 +475,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1441.5</v>
+        <v>1668.65</v>
       </c>
       <c r="E2" t="n">
-        <v>1513.55</v>
+        <v>1752.05</v>
       </c>
       <c r="F2" t="n">
         <v>5</v>
@@ -490,7 +490,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jet Airways</t>
+          <t>National Plywood Ind</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -499,10 +499,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>108.05</v>
+        <v>5.2</v>
       </c>
       <c r="E3" t="n">
-        <v>113.45</v>
+        <v>5.46</v>
       </c>
       <c r="F3" t="n">
         <v>5</v>
@@ -514,7 +514,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>C &amp; C Constructions</t>
+          <t>Kobo Biotech</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -523,13 +523,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>5.41</v>
+        <v>7.19</v>
       </c>
       <c r="E4" t="n">
-        <v>5.68</v>
+        <v>7.54</v>
       </c>
       <c r="F4" t="n">
-        <v>4.99</v>
+        <v>4.87</v>
       </c>
     </row>
     <row r="5">
@@ -538,7 +538,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>IL&amp;FS Transportation</t>
+          <t>Tantia Constructions</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -547,13 +547,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.61</v>
+        <v>2.1</v>
       </c>
       <c r="E5" t="n">
-        <v>2.74</v>
+        <v>2.2</v>
       </c>
       <c r="F5" t="n">
-        <v>4.98</v>
+        <v>4.76</v>
       </c>
     </row>
     <row r="6">
@@ -562,7 +562,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Kobo Biotech</t>
+          <t>CLC Industries</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -571,13 +571,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>6.22</v>
+        <v>0.85</v>
       </c>
       <c r="E6" t="n">
-        <v>6.53</v>
+        <v>0.89</v>
       </c>
       <c r="F6" t="n">
-        <v>4.98</v>
+        <v>4.71</v>
       </c>
     </row>
     <row r="7">
@@ -586,7 +586,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Gujarat Metallic</t>
+          <t>Goenka Diamond &amp; Jew</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -595,13 +595,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>12.7</v>
+        <v>1.97</v>
       </c>
       <c r="E7" t="n">
-        <v>13.33</v>
+        <v>2.06</v>
       </c>
       <c r="F7" t="n">
-        <v>4.96</v>
+        <v>4.57</v>
       </c>
     </row>
     <row r="8">
@@ -610,7 +610,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jumbo Bags Ltd</t>
+          <t>Amit Internation</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -619,13 +619,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>8.07</v>
+        <v>2.46</v>
       </c>
       <c r="E8" t="n">
-        <v>8.470000000000001</v>
+        <v>2.55</v>
       </c>
       <c r="F8" t="n">
-        <v>4.96</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="9">
@@ -634,7 +634,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Tantia Constructions</t>
+          <t>Jumbo Bags Ltd</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -643,13 +643,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1.82</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>1.91</v>
+        <v>9.19</v>
       </c>
       <c r="F9" t="n">
-        <v>4.95</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="10">
@@ -658,7 +658,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Easun Reyrolle L</t>
+          <t>Flomic Global Logist</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -667,13 +667,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2.66</v>
+        <v>4.4</v>
       </c>
       <c r="E10" t="n">
-        <v>2.79</v>
+        <v>4.48</v>
       </c>
       <c r="F10" t="n">
-        <v>4.89</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="11">
@@ -682,7 +682,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Govind Rubber</t>
+          <t>HMT Ltd.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -691,13 +691,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>4.98</v>
+        <v>32.75</v>
       </c>
       <c r="E11" t="n">
-        <v>5.22</v>
+        <v>33.2</v>
       </c>
       <c r="F11" t="n">
-        <v>4.82</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="12">
@@ -706,7 +706,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Foundry Fuel Pro</t>
+          <t>Cybermt Infotek</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -715,13 +715,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1.87</v>
+        <v>1.49</v>
       </c>
       <c r="E12" t="n">
-        <v>1.96</v>
+        <v>1.51</v>
       </c>
       <c r="F12" t="n">
-        <v>4.81</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="13">
@@ -739,13 +739,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>5.64</v>
+        <v>5.9</v>
       </c>
       <c r="E13" t="n">
-        <v>5.91</v>
+        <v>5.95</v>
       </c>
       <c r="F13" t="n">
-        <v>4.79</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="14">
@@ -754,7 +754,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bartronics India Ltd</t>
+          <t>Euro Ceramics Ltd.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -763,13 +763,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2.77</v>
+        <v>1.2</v>
       </c>
       <c r="E14" t="n">
-        <v>2.9</v>
+        <v>1.21</v>
       </c>
       <c r="F14" t="n">
-        <v>4.69</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="15">
@@ -778,7 +778,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Indosolar Ltd.</t>
+          <t>Unitech Ltd.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -787,13 +787,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2.57</v>
+        <v>1.76</v>
       </c>
       <c r="E15" t="n">
-        <v>2.69</v>
+        <v>1.77</v>
       </c>
       <c r="F15" t="n">
-        <v>4.67</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="16">
@@ -802,7 +802,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Suraj Products Ltd.</t>
+          <t>Easun Reyrolle L</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -811,469 +811,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>33.3</v>
+        <v>2.89</v>
       </c>
       <c r="E16" t="n">
-        <v>34.85</v>
+        <v>2.9</v>
       </c>
       <c r="F16" t="n">
-        <v>4.65</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Melstar Inform.</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>1.95</v>
-      </c>
-      <c r="E17" t="n">
-        <v>2.04</v>
-      </c>
-      <c r="F17" t="n">
-        <v>4.62</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Jain Studios Ltd</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>1.79</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1.87</v>
-      </c>
-      <c r="F18" t="n">
-        <v>4.47</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Unity Infraprojects</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="F19" t="n">
-        <v>4.4</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>CLC Industries</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="F20" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Diamond Power Infras</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="F21" t="n">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Karuturi Global Ltd.</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="F22" t="n">
-        <v>3.57</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Minolta Finance</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="E23" t="n">
-        <v>1.18</v>
-      </c>
-      <c r="F23" t="n">
-        <v>3.51</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Twinstar Industries</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="F24" t="n">
-        <v>3.45</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Prabhat Technologies</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>328.65</v>
-      </c>
-      <c r="E25" t="n">
-        <v>339</v>
-      </c>
-      <c r="F25" t="n">
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Polo Hotels Limi</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>4.09</v>
-      </c>
-      <c r="E26" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="F26" t="n">
-        <v>2.69</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Boston Leasing</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="E27" t="n">
-        <v>5.85</v>
-      </c>
-      <c r="F27" t="n">
-        <v>2.63</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Cox &amp; Kings L</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="E28" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="F28" t="n">
-        <v>2.36</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Unitech Ltd.</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="E29" t="n">
-        <v>1.84</v>
-      </c>
-      <c r="F29" t="n">
-        <v>2.22</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Mahaveer Infoway Ltd</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>2.57</v>
-      </c>
-      <c r="E30" t="n">
-        <v>2.62</v>
-      </c>
-      <c r="F30" t="n">
-        <v>1.95</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Stratmont Industries</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>10.81</v>
-      </c>
-      <c r="E31" t="n">
-        <v>11.02</v>
-      </c>
-      <c r="F31" t="n">
-        <v>1.94</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Flomic Global Logist</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>4.16</v>
-      </c>
-      <c r="E32" t="n">
-        <v>4.24</v>
-      </c>
-      <c r="F32" t="n">
-        <v>1.92</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Cybermt Infotek</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>1.43</v>
-      </c>
-      <c r="E33" t="n">
-        <v>1.45</v>
-      </c>
-      <c r="F33" t="n">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>HDIL</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>5.83</v>
-      </c>
-      <c r="E34" t="n">
-        <v>5.87</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0.6899999999999999</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Jyoti Structures</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>3.99</v>
-      </c>
-      <c r="E35" t="n">
-        <v>4</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>